<commit_message>
goto pass input to mainframe; prtint_table; log when validation only
</commit_message>
<xml_diff>
--- a/resources/core/runflow.xlsx
+++ b/resources/core/runflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\TestFactory\resources\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D125C2-B4DC-40D1-A15C-840B9C8F795A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCC3180-BF4D-4AE4-8E31-B7FE12A4BA19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="717" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="96">
   <si>
     <t>path</t>
   </si>
@@ -296,6 +296,36 @@
   </si>
   <si>
     <t>--jumpto(Yes,4)</t>
+  </si>
+  <si>
+    <t>--jumpto(Yes, 5)</t>
+  </si>
+  <si>
+    <t>--jumpto(No, 0)</t>
+  </si>
+  <si>
+    <t>wrong path, not jump</t>
+  </si>
+  <si>
+    <t>none path, will jump</t>
+  </si>
+  <si>
+    <t>--jumpto(No, 3)</t>
+  </si>
+  <si>
+    <t>--jumpto(Key, 4)</t>
+  </si>
+  <si>
+    <t>yes_key</t>
+  </si>
+  <si>
+    <t>no_key</t>
+  </si>
+  <si>
+    <t>none path, key is yes, will not jump</t>
+  </si>
+  <si>
+    <t>none path, key is no, will jump</t>
   </si>
 </sst>
 </file>
@@ -1678,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B75A8BA-1B24-4C26-A9DD-B004B98FAC76}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:I3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1689,7 +1719,7 @@
     <col min="1" max="2" width="9.06640625" style="2"/>
     <col min="3" max="3" width="74" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.06640625" style="2"/>
-    <col min="5" max="5" width="12.9296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.06640625" style="2"/>
     <col min="7" max="7" width="15.06640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.59765625" style="2" bestFit="1" customWidth="1"/>
@@ -1765,19 +1795,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>77</v>
+      <c r="E4" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>82</v>
@@ -1796,14 +1820,8 @@
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>84</v>
+      <c r="E5" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>81</v>
@@ -1817,19 +1835,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>77</v>
+      <c r="E6" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>81</v>
@@ -1848,14 +1860,11 @@
       <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>84</v>
+      <c r="E7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>82</v>
@@ -1869,21 +1878,64 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>84</v>
+      <c r="E8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* add --skipby \n * loop by process_cur
</commit_message>
<xml_diff>
--- a/resources/core/runflow.xlsx
+++ b/resources/core/runflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\TestFactory\resources\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCC3180-BF4D-4AE4-8E31-B7FE12A4BA19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C31CB-8B72-4180-BCFB-5623E8612BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="717" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
   <si>
     <t>path</t>
   </si>
@@ -307,12 +307,6 @@
     <t>wrong path, not jump</t>
   </si>
   <si>
-    <t>none path, will jump</t>
-  </si>
-  <si>
-    <t>--jumpto(No, 3)</t>
-  </si>
-  <si>
     <t>--jumpto(Key, 4)</t>
   </si>
   <si>
@@ -326,6 +320,30 @@
   </si>
   <si>
     <t>none path, key is no, will jump</t>
+  </si>
+  <si>
+    <t>--skipby(Key, 4)</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>--jumpto(Key, 0)</t>
+  </si>
+  <si>
+    <t>--skipby(No, 2)</t>
+  </si>
+  <si>
+    <t>none path, will skip to seven</t>
+  </si>
+  <si>
+    <t>--jumpto(Key, 10)</t>
   </si>
 </sst>
 </file>
@@ -1708,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B75A8BA-1B24-4C26-A9DD-B004B98FAC76}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1835,13 +1853,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>81</v>
@@ -1861,10 +1879,10 @@
         <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>82</v>
@@ -1878,16 +1896,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>82</v>
@@ -1907,10 +1925,10 @@
         <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>82</v>
@@ -1924,22 +1942,109 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>82</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* saving, application linked
</commit_message>
<xml_diff>
--- a/resources/core/runflow.xlsx
+++ b/resources/core/runflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\TestFactory\resources\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC5AB1-C54C-4188-85D5-FC3CB8C78F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF460BC-49E0-4E03-8691-8883F4DCF531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="717" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="717" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v2" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="108">
   <si>
     <t>path</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>test that a inactive counter should be off</t>
+  </si>
+  <si>
+    <t>--url</t>
   </si>
 </sst>
 </file>
@@ -846,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E954B1-E325-4E3F-9802-3F6230F70908}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -892,7 +895,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
@@ -1743,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B75A8BA-1B24-4C26-A9DD-B004B98FAC76}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
* add parallel processing
</commit_message>
<xml_diff>
--- a/resources/core/runflow.xlsx
+++ b/resources/core/runflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\TestFactory\resources\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF460BC-49E0-4E03-8691-8883F4DCF531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940D32F8-E86A-4001-A347-BB30692A1679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="717" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="717" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v2" sheetId="11" r:id="rId1"/>
@@ -28,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="107">
   <si>
     <t>path</t>
   </si>
@@ -94,9 +92,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>goto_url</t>
-  </si>
-  <si>
     <t>checkout</t>
   </si>
   <si>
@@ -163,9 +158,6 @@
     <t>goto</t>
   </si>
   <si>
-    <t>wait</t>
-  </si>
-  <si>
     <t>--for(10)</t>
   </si>
   <si>
@@ -362,6 +354,9 @@
   </si>
   <si>
     <t>--url</t>
+  </si>
+  <si>
+    <t>waiting</t>
   </si>
 </sst>
 </file>
@@ -712,22 +707,22 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="2"/>
-    <col min="3" max="3" width="70.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.9296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.06640625" style="2"/>
-    <col min="7" max="7" width="14.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="2" width="9" style="2"/>
+    <col min="3" max="3" width="70.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="2"/>
+    <col min="7" max="7" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -753,18 +748,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -775,19 +770,19 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -798,16 +793,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -815,16 +810,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -832,10 +827,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -849,19 +844,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E954B1-E325-4E3F-9802-3F6230F70908}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.06640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -887,24 +882,24 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -912,39 +907,39 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
       <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -952,19 +947,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -972,16 +967,16 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -993,23 +988,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C409C86-4E1F-4E2A-9807-6806E1666F8F}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="2"/>
-    <col min="3" max="3" width="17.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.06640625" style="2"/>
-    <col min="6" max="6" width="10.46484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9" style="2"/>
+    <col min="3" max="3" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="2"/>
+    <col min="6" max="6" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1032,35 +1027,35 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1068,87 +1063,87 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1166,16 +1161,16 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.73046875" customWidth="1"/>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1198,20 +1193,20 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
@@ -1220,7 +1215,7 @@
       <c r="G2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1228,25 +1223,25 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1254,25 +1249,25 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="G4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1280,28 +1275,28 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1309,216 +1304,216 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="G6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="2" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="I10" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="I13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1535,18 +1530,18 @@
       <selection activeCell="G8" sqref="G8:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="2"/>
+    <col min="1" max="2" width="9" style="2"/>
     <col min="3" max="3" width="74" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.06640625" style="2"/>
-    <col min="7" max="7" width="15.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="2"/>
+    <col min="4" max="6" width="9" style="2"/>
+    <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1569,24 +1564,24 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1594,22 +1589,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1617,25 +1612,25 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1643,25 +1638,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1669,74 +1664,74 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="I8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1750,23 +1745,23 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="2"/>
+    <col min="1" max="2" width="9" style="2"/>
     <col min="3" max="3" width="74" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.06640625" style="2"/>
-    <col min="5" max="5" width="13.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.06640625" style="2"/>
-    <col min="7" max="7" width="15.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="2"/>
+    <col min="4" max="4" width="9" style="2"/>
+    <col min="5" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="2"/>
+    <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1789,35 +1784,35 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1825,19 +1820,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1845,19 +1840,19 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1865,234 +1860,234 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* add: update json
</commit_message>
<xml_diff>
--- a/resources/core/runflow.xlsx
+++ b/resources/core/runflow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\TestFactory\resources\core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\Projects\TestFactory\resources\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940D32F8-E86A-4001-A347-BB30692A1679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DF9CD8-E2C1-4CCE-BA2D-9E87725B6E75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="717" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14865" yWindow="690" windowWidth="21600" windowHeight="11310" tabRatio="717" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v2" sheetId="11" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="test_scrap" sheetId="14" r:id="rId4"/>
     <sheet name="test_disable" sheetId="15" r:id="rId5"/>
     <sheet name="test_jump" sheetId="16" r:id="rId6"/>
+    <sheet name="sme" sheetId="17" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="131">
   <si>
     <t>path</t>
   </si>
@@ -357,6 +358,78 @@
   </si>
   <si>
     <t>waiting</t>
+  </si>
+  <si>
+    <t>#txtLeadName</t>
+  </si>
+  <si>
+    <t>write_input</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>#txtLeadEmail</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>#txtLeadCompanyName</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>#selLeadEmployees</t>
+  </si>
+  <si>
+    <t>num_employee</t>
+  </si>
+  <si>
+    <t>#txtLeadPhoneNum</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>#selLeadContact</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>#txtLeadRemarks</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>button[class*="js-lead-contact-submit"]</t>
+  </si>
+  <si>
+    <t>--submit</t>
+  </si>
+  <si>
+    <t>#chkExistingCustomer</t>
+  </si>
+  <si>
+    <t>click_checkbox</t>
+  </si>
+  <si>
+    <t>#chkContactByConsultant</t>
+  </si>
+  <si>
+    <t>--jumpto(No, 10)</t>
+  </si>
+  <si>
+    <t>--jumpto(No, 12)</t>
+  </si>
+  <si>
+    <t>exist</t>
+  </si>
+  <si>
+    <t>contact</t>
   </si>
 </sst>
 </file>
@@ -988,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C409C86-4E1F-4E2A-9807-6806E1666F8F}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1818,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,4 +2167,268 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C667BA9-FCC1-4268-9598-BAABCA8D2E84}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>